<commit_message>
Add column shipment Type into template
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Export-Invoice.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Export-Invoice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anatolius.thuan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anatolius.thuan\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>JobNo</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>{ETA}</t>
+  </si>
+  <si>
+    <t>Shipment Type</t>
+  </si>
+  <si>
+    <t>{ShipmentType}</t>
   </si>
 </sst>
 </file>
@@ -179,7 +185,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -188,6 +194,17 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -225,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -236,6 +253,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,52 +537,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Y2" sqref="Y2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="30" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="8" width="20" customWidth="1"/>
-    <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="20" width="15" customWidth="1"/>
-    <col min="21" max="24" width="20" customWidth="1"/>
-    <col min="25" max="25" width="15" customWidth="1"/>
-    <col min="26" max="26" width="30" customWidth="1"/>
-    <col min="27" max="27" width="16" customWidth="1"/>
-    <col min="28" max="28" width="14" customWidth="1"/>
-    <col min="29" max="29" width="18" customWidth="1"/>
-    <col min="30" max="30" width="10" customWidth="1"/>
-    <col min="31" max="31" width="12" customWidth="1"/>
-    <col min="32" max="32" width="8" customWidth="1"/>
-    <col min="33" max="33" width="10" customWidth="1"/>
-    <col min="34" max="34" width="14" customWidth="1"/>
-    <col min="35" max="35" width="10" customWidth="1"/>
-    <col min="36" max="36" width="15" customWidth="1"/>
-    <col min="37" max="37" width="12" customWidth="1"/>
-    <col min="38" max="39" width="10" customWidth="1"/>
-    <col min="40" max="40" width="30" customWidth="1"/>
-    <col min="41" max="41" width="15" customWidth="1"/>
-    <col min="42" max="42" width="18" customWidth="1"/>
-    <col min="43" max="43" width="20" customWidth="1"/>
-    <col min="44" max="44" width="25" customWidth="1"/>
+    <col min="4" max="5" width="30" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="9" width="20" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="12" customWidth="1"/>
+    <col min="14" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="16" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
+    <col min="20" max="21" width="15" customWidth="1"/>
+    <col min="22" max="25" width="20" customWidth="1"/>
+    <col min="26" max="26" width="15" customWidth="1"/>
+    <col min="27" max="27" width="30" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
+    <col min="29" max="29" width="14" customWidth="1"/>
+    <col min="30" max="30" width="18" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="12" customWidth="1"/>
+    <col min="33" max="33" width="8" customWidth="1"/>
+    <col min="34" max="34" width="10" customWidth="1"/>
+    <col min="35" max="35" width="14" customWidth="1"/>
+    <col min="36" max="36" width="10" customWidth="1"/>
+    <col min="37" max="37" width="15" customWidth="1"/>
+    <col min="38" max="38" width="12" customWidth="1"/>
+    <col min="39" max="40" width="10" customWidth="1"/>
+    <col min="41" max="41" width="30" customWidth="1"/>
+    <col min="42" max="42" width="15" customWidth="1"/>
+    <col min="43" max="43" width="18" customWidth="1"/>
+    <col min="44" max="44" width="20" customWidth="1"/>
+    <col min="45" max="45" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:26">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,71 +595,74 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -651,151 +675,155 @@
       <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="R2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="5" customFormat="1">
-      <c r="F3" s="6"/>
-      <c r="P3" s="7"/>
+    <row r="3" spans="1:26" s="5" customFormat="1">
+      <c r="G3" s="6"/>
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
-      <c r="U3" s="6"/>
+      <c r="S3" s="7"/>
       <c r="V3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="W3" s="6"/>
       <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" s="5" customFormat="1">
-      <c r="F4" s="6"/>
-      <c r="P4" s="7"/>
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" s="5" customFormat="1">
+      <c r="G4" s="6"/>
       <c r="Q4" s="7"/>
       <c r="R4" s="7"/>
-      <c r="U4" s="6"/>
+      <c r="S4" s="7"/>
       <c r="V4" s="6"/>
-      <c r="X4" s="6"/>
+      <c r="W4" s="6"/>
       <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" s="5" customFormat="1">
-      <c r="F5" s="6"/>
-      <c r="P5" s="7"/>
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" s="5" customFormat="1">
+      <c r="G5" s="6"/>
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
-      <c r="U5" s="6"/>
+      <c r="S5" s="7"/>
       <c r="V5" s="6"/>
-      <c r="X5" s="6"/>
+      <c r="W5" s="6"/>
       <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:25" s="5" customFormat="1">
-      <c r="F6" s="6"/>
-      <c r="P6" s="7"/>
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" s="5" customFormat="1">
+      <c r="G6" s="6"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
-      <c r="U6" s="6"/>
+      <c r="S6" s="7"/>
       <c r="V6" s="6"/>
-      <c r="X6" s="6"/>
+      <c r="W6" s="6"/>
       <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:25" s="5" customFormat="1">
-      <c r="F7" s="6"/>
-      <c r="P7" s="7"/>
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" s="5" customFormat="1">
+      <c r="G7" s="6"/>
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
-      <c r="U7" s="6"/>
+      <c r="S7" s="7"/>
       <c r="V7" s="6"/>
-      <c r="X7" s="6"/>
+      <c r="W7" s="6"/>
       <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:25" s="5" customFormat="1">
-      <c r="F8" s="6"/>
-      <c r="P8" s="7"/>
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" s="5" customFormat="1">
+      <c r="G8" s="6"/>
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
-      <c r="U8" s="6"/>
+      <c r="S8" s="7"/>
       <c r="V8" s="6"/>
-      <c r="X8" s="6"/>
+      <c r="W8" s="6"/>
       <c r="Y8" s="6"/>
-    </row>
-    <row r="9" spans="1:25" s="5" customFormat="1">
-      <c r="F9" s="6"/>
-      <c r="P9" s="7"/>
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" s="5" customFormat="1">
+      <c r="G9" s="6"/>
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
-      <c r="U9" s="6"/>
+      <c r="S9" s="7"/>
       <c r="V9" s="6"/>
-      <c r="X9" s="6"/>
+      <c r="W9" s="6"/>
       <c r="Y9" s="6"/>
-    </row>
-    <row r="10" spans="1:25" s="5" customFormat="1">
-      <c r="F10" s="6"/>
-      <c r="P10" s="7"/>
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" s="5" customFormat="1">
+      <c r="G10" s="6"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
-      <c r="U10" s="6"/>
+      <c r="S10" s="7"/>
       <c r="V10" s="6"/>
-      <c r="X10" s="6"/>
+      <c r="W10" s="6"/>
       <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change format money, change get sm on request #19509
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Export-Invoice.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/Export-Invoice.xlsx
@@ -541,7 +541,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -714,10 +714,10 @@
       <c r="Q2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>42</v>
       </c>
       <c r="T2" s="2" t="s">

</xml_diff>